<commit_message>
fix: choice questions and excel 3
</commit_message>
<xml_diff>
--- a/media/upload_xlsx/半年销售统计表.xlsx
+++ b/media/upload_xlsx/半年销售统计表.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\class\quiz-system\excel题目\excel-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\quiz-system\office考试系统\exam-office-2021-11-30\media\upload_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5705018C-E06C-45A7-96F3-27532E34CDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="-345" windowWidth="10425" windowHeight="6840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -392,11 +393,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -429,16 +430,41 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -466,45 +492,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -515,341 +563,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -860,38 +623,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:K46" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A2:K46">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="11">
-    <tableColumn id="1" name="员工编号" dataDxfId="10"/>
-    <tableColumn id="2" name="姓名" dataDxfId="9"/>
-    <tableColumn id="3" name="销售团队" dataDxfId="8"/>
-    <tableColumn id="4" name="一月份" dataDxfId="7"/>
-    <tableColumn id="5" name="二月份" dataDxfId="6"/>
-    <tableColumn id="6" name="三月份" dataDxfId="5"/>
-    <tableColumn id="7" name="四月份" dataDxfId="4"/>
-    <tableColumn id="8" name="五月分" dataDxfId="3"/>
-    <tableColumn id="9" name="六月份" dataDxfId="2"/>
-    <tableColumn id="10" name="个人销售总计" dataDxfId="1"/>
-    <tableColumn id="11" name="销售排名" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -970,6 +701,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1005,6 +753,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1180,11 +945,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1193,1425 +958,1425 @@
     <col min="2" max="2" width="9.625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="9" width="15.625" customWidth="1"/>
-    <col min="10" max="10" width="21.75" style="10" customWidth="1"/>
+    <col min="10" max="10" width="21.75" style="2" customWidth="1"/>
     <col min="11" max="11" width="12.375" customWidth="1"/>
     <col min="12" max="12" width="1.875" customWidth="1"/>
     <col min="13" max="13" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="45" customHeight="1" thickTop="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:11" s="1" customFormat="1" thickTop="1">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="11">
         <v>66500</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="11">
         <v>92500</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="11">
         <v>95500</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="11">
         <v>98000</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="11">
         <v>86500</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="11">
         <v>71000</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A4" s="4" t="s">
+      <c r="J3" s="11"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="14">
         <v>73500</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="14">
         <v>91500</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="14">
         <v>64500</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="14">
         <v>93500</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="14">
         <v>84000</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="14">
         <v>87000</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A5" s="4" t="s">
+      <c r="J4" s="14"/>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="17">
         <v>75500</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="17">
         <v>62500</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="17">
         <v>87000</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="17">
         <v>94500</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="17">
         <v>78000</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="17">
         <v>91000</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A6" s="4" t="s">
+      <c r="J5" s="17"/>
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="14">
         <v>79500</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="14">
         <v>98500</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="14">
         <v>68000</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="14">
         <v>100000</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="14">
         <v>96000</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="14">
         <v>66000</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A7" s="4" t="s">
+      <c r="J6" s="14"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="17">
         <v>82050</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="17">
         <v>63500</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="17">
         <v>90500</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="17">
         <v>97000</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="17">
         <v>65150</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="17">
         <v>99000</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A8" s="4" t="s">
+      <c r="J7" s="17"/>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="14">
         <v>82500</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="14">
         <v>78000</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="14">
         <v>81000</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="14">
         <v>96500</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="14">
         <v>96500</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="14">
         <v>57000</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A9" s="4" t="s">
+      <c r="J8" s="14"/>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="17">
         <v>84500</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="17">
         <v>71000</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="17">
         <v>99500</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="17">
         <v>89500</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="17">
         <v>84500</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="17">
         <v>58000</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A10" s="4" t="s">
+      <c r="J9" s="17"/>
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="14">
         <v>87500</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="14">
         <v>63500</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="14">
         <v>67500</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="14">
         <v>98500</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="14">
         <v>78500</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="14">
         <v>94000</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A11" s="4" t="s">
+      <c r="J10" s="14"/>
+      <c r="K10" s="13"/>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="17">
         <v>88000</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="17">
         <v>82500</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="17">
         <v>83000</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="17">
         <v>75500</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="17">
         <v>62000</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="17">
         <v>85000</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A12" s="4" t="s">
+      <c r="J11" s="17"/>
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="14">
         <v>92000</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="14">
         <v>64000</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="14">
         <v>97000</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="14">
         <v>93000</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="14">
         <v>75000</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="14">
         <v>93000</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A13" s="4" t="s">
+      <c r="J12" s="14"/>
+      <c r="K12" s="13"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A13" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="17">
         <v>93000</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="17">
         <v>71500</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="17">
         <v>92000</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="17">
         <v>96500</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="17">
         <v>87000</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="17">
         <v>61000</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A14" s="4" t="s">
+      <c r="J13" s="17"/>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="14">
         <v>93050</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="14">
         <v>85500</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="14">
         <v>77000</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="14">
         <v>81000</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="14">
         <v>95000</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="14">
         <v>78000</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A15" s="4" t="s">
+      <c r="J14" s="14"/>
+      <c r="K14" s="13"/>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A15" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="17">
         <v>96000</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="17">
         <v>72500</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="17">
         <v>100000</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="17">
         <v>86000</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="17">
         <v>62000</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="17">
         <v>87500</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A16" s="4" t="s">
+      <c r="J15" s="17"/>
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A16" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="14">
         <v>96500</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="14">
         <v>86500</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="14">
         <v>90500</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="14">
         <v>94000</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="14">
         <v>99500</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="14">
         <v>70000</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A17" s="4" t="s">
+      <c r="J16" s="14"/>
+      <c r="K16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="17">
         <v>97500</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="17">
         <v>76000</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="17">
         <v>72000</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="17">
         <v>92500</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="17">
         <v>84500</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="17">
         <v>78000</v>
       </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A18" s="4" t="s">
+      <c r="J17" s="17"/>
+      <c r="K17" s="16"/>
+    </row>
+    <row r="18" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="14">
         <v>56000</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="14">
         <v>77500</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="14">
         <v>85000</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="14">
         <v>83000</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="14">
         <v>74500</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="14">
         <v>79000</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A19" s="4" t="s">
+      <c r="J18" s="14"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A19" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="17">
         <v>58500</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="17">
         <v>90000</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="17">
         <v>88500</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="17">
         <v>97000</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="17">
         <v>72000</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="17">
         <v>65000</v>
       </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" s="3" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="J19" s="17"/>
+      <c r="K19" s="16"/>
+    </row>
+    <row r="20" spans="1:11" s="1" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="14">
         <v>63000</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="14">
         <v>99500</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="14">
         <v>78500</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="14">
         <v>63150</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="14">
         <v>79500</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="14">
         <v>65500</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A21" s="4" t="s">
+      <c r="J20" s="14"/>
+      <c r="K20" s="13"/>
+    </row>
+    <row r="21" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A21" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="17">
         <v>69000</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="17">
         <v>89500</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="17">
         <v>92500</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="17">
         <v>73000</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="17">
         <v>58500</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="17">
         <v>96500</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A22" s="4" t="s">
+      <c r="J21" s="17"/>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="14">
         <v>72500</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="14">
         <v>74500</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="14">
         <v>60500</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="14">
         <v>87000</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="14">
         <v>77000</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="14">
         <v>78000</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A23" s="4" t="s">
+      <c r="J22" s="14"/>
+      <c r="K22" s="13"/>
+    </row>
+    <row r="23" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A23" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="17">
         <v>74000</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="17">
         <v>72500</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="17">
         <v>67000</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="17">
         <v>94000</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="17">
         <v>78000</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="17">
         <v>90000</v>
       </c>
-      <c r="J23" s="9"/>
-      <c r="K23" s="5"/>
-    </row>
-    <row r="24" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A24" s="4" t="s">
+      <c r="J23" s="17"/>
+      <c r="K23" s="16"/>
+    </row>
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="14">
         <v>75500</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="14">
         <v>72500</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="14">
         <v>75000</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="14">
         <v>92000</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="14">
         <v>86000</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="14">
         <v>55000</v>
       </c>
-      <c r="J24" s="9"/>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="25" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A25" s="4" t="s">
+      <c r="J24" s="14"/>
+      <c r="K24" s="13"/>
+    </row>
+    <row r="25" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A25" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="17">
         <v>76500</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="17">
         <v>70000</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="17">
         <v>64000</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="17">
         <v>75000</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="17">
         <v>87000</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="17">
         <v>78000</v>
       </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="5"/>
-    </row>
-    <row r="26" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A26" s="4" t="s">
+      <c r="J25" s="17"/>
+      <c r="K25" s="16"/>
+    </row>
+    <row r="26" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A26" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="14">
         <v>77000</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="14">
         <v>60500</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="14">
         <v>66050</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="14">
         <v>84000</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="14">
         <v>98000</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="14">
         <v>93000</v>
       </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A27" s="4" t="s">
+      <c r="J26" s="14"/>
+      <c r="K26" s="13"/>
+    </row>
+    <row r="27" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A27" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="17">
         <v>80500</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="17">
         <v>96000</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="17">
         <v>72000</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="17">
         <v>66000</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="17">
         <v>61000</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="17">
         <v>85000</v>
       </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A28" s="4" t="s">
+      <c r="J27" s="17"/>
+      <c r="K27" s="16"/>
+    </row>
+    <row r="28" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A28" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="14">
         <v>83500</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="14">
         <v>78500</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="14">
         <v>70500</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="14">
         <v>100000</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="14">
         <v>68150</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="14">
         <v>69000</v>
       </c>
-      <c r="J28" s="9"/>
-      <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A29" s="4" t="s">
+      <c r="J28" s="14"/>
+      <c r="K28" s="13"/>
+    </row>
+    <row r="29" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A29" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="17">
         <v>84500</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="17">
         <v>78500</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="17">
         <v>87500</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="17">
         <v>64500</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="17">
         <v>72000</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="17">
         <v>76500</v>
       </c>
-      <c r="J29" s="9"/>
-      <c r="K29" s="5"/>
-    </row>
-    <row r="30" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A30" s="4" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="16"/>
+    </row>
+    <row r="30" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A30" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="14">
         <v>92500</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="14">
         <v>93500</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="14">
         <v>77000</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="14">
         <v>73000</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="14">
         <v>57000</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="14">
         <v>84000</v>
       </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="5"/>
-    </row>
-    <row r="31" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A31" s="4" t="s">
+      <c r="J30" s="14"/>
+      <c r="K30" s="13"/>
+    </row>
+    <row r="31" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A31" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="17">
         <v>95000</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="17">
         <v>95000</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="17">
         <v>70000</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="17">
         <v>89500</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="17">
         <v>61150</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="17">
         <v>61500</v>
       </c>
-      <c r="J31" s="9"/>
-      <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A32" s="4" t="s">
+      <c r="J31" s="17"/>
+      <c r="K31" s="16"/>
+    </row>
+    <row r="32" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A32" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="14">
         <v>97000</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="14">
         <v>75500</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="14">
         <v>73000</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="14">
         <v>81000</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="14">
         <v>66000</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="14">
         <v>76000</v>
       </c>
-      <c r="J32" s="9"/>
-      <c r="K32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A33" s="4" t="s">
+      <c r="J32" s="14"/>
+      <c r="K32" s="13"/>
+    </row>
+    <row r="33" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A33" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="17">
         <v>62500</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="17">
         <v>76000</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="17">
         <v>57000</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="17">
         <v>67500</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="17">
         <v>88000</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="17">
         <v>84500</v>
       </c>
-      <c r="J33" s="9"/>
-      <c r="K33" s="5"/>
-    </row>
-    <row r="34" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A34" s="4" t="s">
+      <c r="J33" s="17"/>
+      <c r="K33" s="16"/>
+    </row>
+    <row r="34" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A34" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="14">
         <v>62500</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="14">
         <v>57500</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="14">
         <v>85000</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="14">
         <v>59000</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="14">
         <v>79000</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="14">
         <v>61500</v>
       </c>
-      <c r="J34" s="9"/>
-      <c r="K34" s="5"/>
-    </row>
-    <row r="35" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A35" s="4" t="s">
+      <c r="J34" s="14"/>
+      <c r="K34" s="13"/>
+    </row>
+    <row r="35" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A35" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="17">
         <v>63500</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="17">
         <v>73000</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="17">
         <v>65000</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="17">
         <v>95000</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="17">
         <v>75500</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="17">
         <v>61000</v>
       </c>
-      <c r="J35" s="9"/>
-      <c r="K35" s="5"/>
-    </row>
-    <row r="36" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A36" s="4" t="s">
+      <c r="J35" s="17"/>
+      <c r="K35" s="16"/>
+    </row>
+    <row r="36" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A36" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="14">
         <v>68000</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="14">
         <v>97500</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="14">
         <v>61000</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="14">
         <v>57000</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="14">
         <v>60000</v>
       </c>
-      <c r="I36" s="7">
+      <c r="I36" s="14">
         <v>85000</v>
       </c>
-      <c r="J36" s="9"/>
-      <c r="K36" s="5"/>
-    </row>
-    <row r="37" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A37" s="4" t="s">
+      <c r="J36" s="14"/>
+      <c r="K36" s="13"/>
+    </row>
+    <row r="37" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A37" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="17">
         <v>71500</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="17">
         <v>61500</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="17">
         <v>82000</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="17">
         <v>57500</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="17">
         <v>57000</v>
       </c>
-      <c r="I37" s="7">
+      <c r="I37" s="17">
         <v>85000</v>
       </c>
-      <c r="J37" s="9"/>
-      <c r="K37" s="5"/>
-    </row>
-    <row r="38" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A38" s="4" t="s">
+      <c r="J37" s="17"/>
+      <c r="K37" s="16"/>
+    </row>
+    <row r="38" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A38" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="14">
         <v>71500</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="14">
         <v>59500</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="14">
         <v>88000</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="14">
         <v>63000</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38" s="14">
         <v>88000</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="14">
         <v>60500</v>
       </c>
-      <c r="J38" s="9"/>
-      <c r="K38" s="5"/>
-    </row>
-    <row r="39" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A39" s="4" t="s">
+      <c r="J38" s="14"/>
+      <c r="K38" s="13"/>
+    </row>
+    <row r="39" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A39" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="17">
         <v>75000</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="17">
         <v>71000</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="17">
         <v>86000</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="17">
         <v>60500</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="17">
         <v>60000</v>
       </c>
-      <c r="I39" s="7">
+      <c r="I39" s="17">
         <v>85000</v>
       </c>
-      <c r="J39" s="9"/>
-      <c r="K39" s="5"/>
-    </row>
-    <row r="40" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A40" s="4" t="s">
+      <c r="J39" s="17"/>
+      <c r="K39" s="16"/>
+    </row>
+    <row r="40" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A40" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="14">
         <v>75500</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="14">
         <v>60500</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="14">
         <v>85000</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40" s="14">
         <v>57000</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="14">
         <v>76000</v>
       </c>
-      <c r="I40" s="7">
+      <c r="I40" s="14">
         <v>83000</v>
       </c>
-      <c r="J40" s="9"/>
-      <c r="K40" s="5"/>
-    </row>
-    <row r="41" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A41" s="4" t="s">
+      <c r="J40" s="14"/>
+      <c r="K40" s="13"/>
+    </row>
+    <row r="41" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A41" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="17">
         <v>76000</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="17">
         <v>63500</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="17">
         <v>84000</v>
       </c>
-      <c r="G41" s="7">
+      <c r="G41" s="17">
         <v>81000</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="17">
         <v>65000</v>
       </c>
-      <c r="I41" s="7">
+      <c r="I41" s="17">
         <v>62000</v>
       </c>
-      <c r="J41" s="9"/>
-      <c r="K41" s="5"/>
-    </row>
-    <row r="42" spans="1:11" s="3" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A42" s="4" t="s">
+      <c r="J41" s="17"/>
+      <c r="K41" s="16"/>
+    </row>
+    <row r="42" spans="1:11" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A42" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="14">
         <v>81000</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="14">
         <v>55500</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="14">
         <v>61000</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G42" s="14">
         <v>91500</v>
       </c>
-      <c r="H42" s="7">
+      <c r="H42" s="14">
         <v>81000</v>
       </c>
-      <c r="I42" s="7">
+      <c r="I42" s="14">
         <v>59000</v>
       </c>
-      <c r="J42" s="9"/>
-      <c r="K42" s="5"/>
-    </row>
-    <row r="43" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A43" s="4" t="s">
+      <c r="J42" s="14"/>
+      <c r="K42" s="13"/>
+    </row>
+    <row r="43" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A43" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="17">
         <v>85500</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="17">
         <v>64500</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="17">
         <v>74000</v>
       </c>
-      <c r="G43" s="7">
+      <c r="G43" s="17">
         <v>78500</v>
       </c>
-      <c r="H43" s="7">
+      <c r="H43" s="17">
         <v>64000</v>
       </c>
-      <c r="I43" s="7">
+      <c r="I43" s="17">
         <v>76000</v>
       </c>
-      <c r="J43" s="9"/>
-      <c r="K43" s="5"/>
-    </row>
-    <row r="44" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A44" s="4" t="s">
+      <c r="J43" s="17"/>
+      <c r="K43" s="16"/>
+    </row>
+    <row r="44" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A44" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="14">
         <v>86500</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="14">
         <v>65500</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F44" s="14">
         <v>67500</v>
       </c>
-      <c r="G44" s="7">
+      <c r="G44" s="14">
         <v>70500</v>
       </c>
-      <c r="H44" s="7">
+      <c r="H44" s="14">
         <v>62000</v>
       </c>
-      <c r="I44" s="7">
+      <c r="I44" s="14">
         <v>73000</v>
       </c>
-      <c r="J44" s="9"/>
-      <c r="K44" s="5"/>
-    </row>
-    <row r="45" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A45" s="4" t="s">
+      <c r="J44" s="14"/>
+      <c r="K44" s="13"/>
+    </row>
+    <row r="45" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A45" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="17">
         <v>94000</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="17">
         <v>68050</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F45" s="17">
         <v>78000</v>
       </c>
-      <c r="G45" s="7">
+      <c r="G45" s="17">
         <v>60500</v>
       </c>
-      <c r="H45" s="7">
+      <c r="H45" s="17">
         <v>76000</v>
       </c>
-      <c r="I45" s="7">
+      <c r="I45" s="17">
         <v>67000</v>
       </c>
-      <c r="J45" s="9"/>
-      <c r="K45" s="5"/>
-    </row>
-    <row r="46" spans="1:11" s="3" customFormat="1" ht="13.5">
-      <c r="A46" s="4" t="s">
+      <c r="J45" s="17"/>
+      <c r="K45" s="16"/>
+    </row>
+    <row r="46" spans="1:11" s="1" customFormat="1" ht="13.5">
+      <c r="A46" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="14">
         <v>96500</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="14">
         <v>74500</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="14">
         <v>63000</v>
       </c>
-      <c r="G46" s="7">
+      <c r="G46" s="14">
         <v>66000</v>
       </c>
-      <c r="H46" s="7">
+      <c r="H46" s="14">
         <v>71000</v>
       </c>
-      <c r="I46" s="7">
+      <c r="I46" s="14">
         <v>69000</v>
       </c>
-      <c r="J46" s="9"/>
-      <c r="K46" s="5"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="13"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -2619,8 +2384,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>